<commit_message>
Fin du code et ajout de la doc
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\BatailleNavale\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierr_u9c72gq\OneDrive\Bureau\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD975B15-95D9-40EC-9667-B305FFA7454E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5805"/>
+    <workbookView xWindow="2210" yWindow="540" windowWidth="14400" windowHeight="8830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t xml:space="preserve">Jour </t>
   </si>
@@ -99,12 +100,39 @@
   </si>
   <si>
     <t>Ajout d'un décompte affichant le nombre de bateaux restant</t>
+  </si>
+  <si>
+    <t>Introduction du S.M.A.R.T</t>
+  </si>
+  <si>
+    <t>Fin de l'option d'écriture dans des fichiers externe au code</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>Fin de l'option de lecture dans des fichiers externe au code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Théorie teste </t>
+  </si>
+  <si>
+    <t>Théorie sur la documentation</t>
+  </si>
+  <si>
+    <t>3h30</t>
+  </si>
+  <si>
+    <t>Création de la documentation</t>
+  </si>
+  <si>
+    <t>Fin de la version 1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,23 +475,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.25" customWidth="1"/>
     <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="13.08203125" customWidth="1"/>
     <col min="5" max="5" width="64.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44242</v>
       </c>
@@ -497,7 +525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44244</v>
       </c>
@@ -514,7 +542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44245</v>
       </c>
@@ -531,7 +559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44246</v>
       </c>
@@ -548,7 +576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44256</v>
       </c>
@@ -565,7 +593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44258</v>
       </c>
@@ -582,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44259</v>
       </c>
@@ -599,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44263</v>
       </c>
@@ -616,7 +644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44265</v>
       </c>
@@ -633,7 +661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44266</v>
       </c>
@@ -650,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44266</v>
       </c>
@@ -667,7 +695,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44267</v>
       </c>
@@ -676,6 +704,116 @@
       </c>
       <c r="E13" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>44272</v>
+      </c>
+      <c r="B14" s="4">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B17" s="4">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44288</v>
+      </c>
+      <c r="B19" s="4">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44288</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>